<commit_message>
ver.2 finalized ver from Kwak
</commit_message>
<xml_diff>
--- a/result_df_output.xlsx
+++ b/result_df_output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN304"/>
+  <dimension ref="A1:AN305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49499,6 +49499,78 @@
         <v>0</v>
       </c>
     </row>
+    <row r="305">
+      <c r="A305" t="inlineStr"/>
+      <c r="B305" t="inlineStr"/>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+      <c r="G305" t="inlineStr"/>
+      <c r="H305" t="inlineStr"/>
+      <c r="I305" t="inlineStr"/>
+      <c r="J305" t="inlineStr"/>
+      <c r="K305" t="inlineStr"/>
+      <c r="L305" t="inlineStr"/>
+      <c r="M305" t="inlineStr"/>
+      <c r="N305" t="inlineStr"/>
+      <c r="O305" t="n">
+        <v>2</v>
+      </c>
+      <c r="P305" t="inlineStr"/>
+      <c r="Q305" t="inlineStr"/>
+      <c r="R305" t="inlineStr"/>
+      <c r="S305" t="inlineStr"/>
+      <c r="T305" t="inlineStr"/>
+      <c r="U305" t="inlineStr"/>
+      <c r="V305" t="inlineStr"/>
+      <c r="W305" t="inlineStr"/>
+      <c r="X305" t="inlineStr"/>
+      <c r="Y305" t="inlineStr"/>
+      <c r="Z305" t="inlineStr"/>
+      <c r="AA305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN305" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>